<commit_message>
update BOM_AxxSolder_V2_0-xlsx with cleaner links
</commit_message>
<xml_diff>
--- a/PCB/AxxSolder/bom/BOM_AxxSolder_V2_0.xlsx
+++ b/PCB/AxxSolder/bom/BOM_AxxSolder_V2_0.xlsx
@@ -15,6 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -611,9 +612,6 @@
     <t>TOTAL Sum with genuine JBC handle and stand</t>
   </si>
   <si>
-    <t>https://www.aliexpress.com/item/1005005736571669.html?spm=a2g0o.productlist.main.13.40961309ZBPluL&amp;algo_pvid=2a86f647-a168-4c57-b57f-0bc3f2028986&amp;algo_exp_id=2a86f647-a168-4c57-b57f-0bc3f2028986-6&amp;pdp_npi=4%40dis%21SEK%2161.31%2140.42%21%21%215.40%21%21%4021038eda16963400910536291e39e5%2112000034161490814%21sea%21SE%210%21AB&amp;curPageLogUid=y8WcCX6oO4rW</t>
-  </si>
-  <si>
     <t>SUM JBC stand and handle</t>
   </si>
   <si>
@@ -629,9 +627,6 @@
     <t>T210 handle piece + 3 tips</t>
   </si>
   <si>
-    <t>https://www.aliexpress.com/item/1005005857983522.html?spm=a2g0o.productlist.main.7.547958eeyrBoxm&amp;algo_pvid=489fedfe-437e-43f1-9cf0-0189d2572bb7&amp;algo_exp_id=489fedfe-437e-43f1-9cf0-0189d2572bb7-3&amp;pdp_npi=4%40dis%21SEK%2177.43%2148.03%21%21%216.82%21%21%40211b88ee16963403808713272e3668%2112000034597993046%21sea%21SE%210%21AB&amp;curPageLogUid=2DDVGU71yADG</t>
-  </si>
-  <si>
     <t>TOTAL Sum with non-brand handle and stand</t>
   </si>
   <si>
@@ -648,6 +643,12 @@
   </si>
   <si>
     <t>WARNING: NOT tested, but does probably work</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/1005005857983522.html</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/1005005736571669.html</t>
   </si>
 </sst>
 </file>
@@ -658,7 +659,7 @@
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;kr&quot;_-;\-* #,##0.00\ &quot;kr&quot;_-;_-* &quot;-&quot;??\ &quot;kr&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -690,15 +691,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -755,7 +747,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -778,37 +770,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="164" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1087,10 +1090,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M13" sqref="M12:M13"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="J58" sqref="J58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1102,7 +1108,7 @@
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24.5703125" customWidth="1"/>
-    <col min="8" max="8" width="69.140625" customWidth="1"/>
+    <col min="8" max="8" width="111" customWidth="1"/>
     <col min="9" max="9" width="49.5703125" customWidth="1"/>
     <col min="10" max="10" width="38" customWidth="1"/>
     <col min="11" max="11" width="26.5703125" customWidth="1"/>
@@ -1112,8 +1118,8 @@
       <c r="A1" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B1" s="15" t="s">
-        <v>206</v>
+      <c r="B1" s="9" t="s">
+        <v>204</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -1142,10 +1148,10 @@
         <v>141</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2" t="s">
@@ -1159,1059 +1165,1099 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="14">
         <v>5</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="15">
         <v>0.89300000000000002</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="16">
         <f>E3*F3</f>
         <v>4.4649999999999999</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="14" t="s">
         <v>143</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="14" t="s">
         <v>9</v>
       </c>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="17">
         <v>12</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="18">
         <v>9.2999999999999999E-2</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="19">
         <f t="shared" ref="G4:G34" si="0">E4*F4</f>
         <v>1.1160000000000001</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="17" t="s">
         <v>9</v>
       </c>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="17">
         <v>3</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="18">
         <v>0.88400000000000001</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="19">
         <f t="shared" si="0"/>
         <v>2.6520000000000001</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="17" t="s">
         <v>144</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="17" t="s">
         <v>9</v>
       </c>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="17">
         <v>2</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="18">
         <v>9.2999999999999999E-2</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="19">
         <f t="shared" si="0"/>
         <v>0.186</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="17" t="s">
         <v>9</v>
       </c>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7" s="4">
+      <c r="E7" s="17">
+        <v>1</v>
+      </c>
+      <c r="F7" s="18">
         <v>1.1599999999999999</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="19">
         <f t="shared" si="0"/>
         <v>1.1599999999999999</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="17" t="s">
         <v>146</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K7" s="17" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="17">
         <v>5</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="18">
         <v>0.26</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="19">
         <f t="shared" si="0"/>
         <v>1.3</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="17" t="s">
         <v>9</v>
       </c>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9" s="4">
+      <c r="E9" s="17">
+        <v>1</v>
+      </c>
+      <c r="F9" s="18">
         <v>0.41899999999999998</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="19">
         <f t="shared" si="0"/>
         <v>0.41899999999999998</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="17" t="s">
         <v>148</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K9" s="17" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10" s="4">
+      <c r="E10" s="17">
+        <v>1</v>
+      </c>
+      <c r="F10" s="18">
         <v>12.9</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="19">
         <f t="shared" si="0"/>
         <v>12.9</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="17" t="s">
         <v>149</v>
       </c>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="F11" s="4">
+      <c r="E11" s="17">
+        <v>1</v>
+      </c>
+      <c r="F11" s="18">
         <v>0.44600000000000001</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11" s="19">
         <f t="shared" si="0"/>
         <v>0.44600000000000001</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I11" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J11" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K11" s="17" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12" s="4">
+      <c r="E12" s="17">
+        <v>1</v>
+      </c>
+      <c r="F12" s="18">
         <v>0.58599999999999997</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12" s="19">
         <f t="shared" si="0"/>
         <v>0.58599999999999997</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="H12" s="17" t="s">
         <v>151</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I12" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J12" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="K12" t="s">
+      <c r="K12" s="17" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13" s="4">
+      <c r="E13" s="17">
+        <v>1</v>
+      </c>
+      <c r="F13" s="18">
         <v>1.1000000000000001</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G13" s="19">
         <f t="shared" si="0"/>
         <v>1.1000000000000001</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13" s="17" t="s">
         <v>152</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I13" s="17" t="s">
         <v>9</v>
       </c>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-      <c r="F14" s="4">
+      <c r="E14" s="17">
+        <v>1</v>
+      </c>
+      <c r="F14" s="18">
         <v>5.72</v>
       </c>
-      <c r="G14" s="5">
+      <c r="G14" s="19">
         <f t="shared" si="0"/>
         <v>5.72</v>
       </c>
-      <c r="H14" s="3" t="s">
+      <c r="H14" s="17" t="s">
         <v>153</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I14" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="J14" t="s">
+      <c r="J14" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="K14" t="s">
+      <c r="K14" s="17" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
-      <c r="F15" s="4">
+      <c r="E15" s="17">
+        <v>1</v>
+      </c>
+      <c r="F15" s="18">
         <v>6.45</v>
       </c>
-      <c r="G15" s="5">
+      <c r="G15" s="19">
         <f t="shared" si="0"/>
         <v>6.45</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H15" s="17" t="s">
         <v>154</v>
       </c>
-      <c r="I15" t="s">
+      <c r="I15" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="J15" t="s">
+      <c r="J15" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="K15" t="s">
+      <c r="K15" s="17" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-      <c r="F16" s="4">
+      <c r="E16" s="17">
+        <v>1</v>
+      </c>
+      <c r="F16" s="18">
         <v>0.54900000000000004</v>
       </c>
-      <c r="G16" s="5">
+      <c r="G16" s="19">
         <f t="shared" si="0"/>
         <v>0.54900000000000004</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="H16" s="17" t="s">
         <v>155</v>
       </c>
-      <c r="I16" t="s">
+      <c r="I16" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="J16" t="s">
+      <c r="J16" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="K16" t="s">
+      <c r="K16" s="17" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-      <c r="F17" s="4">
+      <c r="E17" s="17">
+        <v>1</v>
+      </c>
+      <c r="F17" s="18">
         <v>3.78</v>
       </c>
-      <c r="G17" s="5">
+      <c r="G17" s="19">
         <f t="shared" si="0"/>
         <v>3.78</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H17" s="17" t="s">
         <v>156</v>
       </c>
-      <c r="I17" t="s">
+      <c r="I17" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="J17" t="s">
+      <c r="J17" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="K17" t="s">
+      <c r="K17" s="17" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-      <c r="F18" s="4">
+      <c r="E18" s="17">
+        <v>1</v>
+      </c>
+      <c r="F18" s="18">
         <v>2.99</v>
       </c>
-      <c r="G18" s="5">
+      <c r="G18" s="19">
         <f t="shared" si="0"/>
         <v>2.99</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H18" s="17" t="s">
         <v>157</v>
       </c>
-      <c r="I18" t="s">
+      <c r="I18" s="17" t="s">
         <v>9</v>
       </c>
+      <c r="J18" s="17"/>
+      <c r="K18" s="17"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="E19">
-        <v>1</v>
-      </c>
-      <c r="F19" s="4">
+      <c r="E19" s="17">
+        <v>1</v>
+      </c>
+      <c r="F19" s="18">
         <v>1.5</v>
       </c>
-      <c r="G19" s="5">
+      <c r="G19" s="19">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H19" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="I19" t="s">
+      <c r="I19" s="17" t="s">
         <v>9</v>
       </c>
+      <c r="J19" s="17"/>
+      <c r="K19" s="17"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-      <c r="F20" s="4">
+      <c r="E20" s="17">
+        <v>1</v>
+      </c>
+      <c r="F20" s="18">
         <v>2.71</v>
       </c>
-      <c r="G20" s="5">
+      <c r="G20" s="19">
         <f t="shared" si="0"/>
         <v>2.71</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H20" s="17" t="s">
         <v>159</v>
       </c>
-      <c r="I20" t="s">
+      <c r="I20" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="J20" t="s">
+      <c r="J20" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="K20" t="s">
+      <c r="K20" s="17" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="E21">
-        <v>1</v>
-      </c>
-      <c r="F21" s="4">
+      <c r="E21" s="17">
+        <v>1</v>
+      </c>
+      <c r="F21" s="18">
         <v>0.83699999999999997</v>
       </c>
-      <c r="G21" s="5">
+      <c r="G21" s="19">
         <f t="shared" si="0"/>
         <v>0.83699999999999997</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H21" s="17" t="s">
         <v>160</v>
       </c>
-      <c r="I21" t="s">
+      <c r="I21" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="J21" t="s">
+      <c r="J21" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="K21" t="s">
+      <c r="K21" s="17" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="E22">
-        <v>1</v>
-      </c>
-      <c r="F22" s="4">
+      <c r="E22" s="17">
+        <v>1</v>
+      </c>
+      <c r="F22" s="18">
         <v>10.93</v>
       </c>
-      <c r="G22" s="5">
+      <c r="G22" s="19">
         <f t="shared" si="0"/>
         <v>10.93</v>
       </c>
-      <c r="H22" t="s">
+      <c r="H22" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="I22" t="s">
+      <c r="I22" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="J22" t="s">
+      <c r="J22" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="K22" t="s">
+      <c r="K22" s="17" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="E23">
-        <v>1</v>
-      </c>
-      <c r="F23" s="4">
+      <c r="E23" s="17">
+        <v>1</v>
+      </c>
+      <c r="F23" s="18">
         <v>0.17699999999999999</v>
       </c>
-      <c r="G23" s="5">
+      <c r="G23" s="19">
         <f t="shared" si="0"/>
         <v>0.17699999999999999</v>
       </c>
-      <c r="H23" t="s">
+      <c r="H23" s="17" t="s">
         <v>162</v>
       </c>
-      <c r="I23" t="s">
+      <c r="I23" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="J23" t="s">
+      <c r="J23" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="K23" t="s">
+      <c r="K23" s="17" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="17">
         <v>6</v>
       </c>
-      <c r="F24" s="4">
+      <c r="F24" s="18">
         <v>0.36299999999999999</v>
       </c>
-      <c r="G24" s="5">
+      <c r="G24" s="19">
         <f t="shared" si="0"/>
         <v>2.1779999999999999</v>
       </c>
-      <c r="H24" t="s">
+      <c r="H24" s="17" t="s">
         <v>181</v>
       </c>
-      <c r="I24" t="s">
+      <c r="I24" s="17" t="s">
         <v>9</v>
       </c>
+      <c r="J24" s="17"/>
+      <c r="K24" s="17"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="E25">
-        <v>1</v>
-      </c>
-      <c r="F25" s="4">
+      <c r="E25" s="17">
+        <v>1</v>
+      </c>
+      <c r="F25" s="18">
         <v>0.186</v>
       </c>
-      <c r="G25" s="5">
+      <c r="G25" s="19">
         <f t="shared" si="0"/>
         <v>0.186</v>
       </c>
-      <c r="H25" s="3" t="s">
+      <c r="H25" s="17" t="s">
         <v>182</v>
       </c>
-      <c r="I25" t="s">
+      <c r="I25" s="17" t="s">
         <v>9</v>
       </c>
+      <c r="J25" s="17"/>
+      <c r="K25" s="17"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="A26" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="E26">
-        <v>1</v>
-      </c>
-      <c r="F26" s="4">
+      <c r="E26" s="17">
+        <v>1</v>
+      </c>
+      <c r="F26" s="18">
         <v>0.27</v>
       </c>
-      <c r="G26" s="5">
+      <c r="G26" s="19">
         <f t="shared" si="0"/>
         <v>0.27</v>
       </c>
-      <c r="H26" t="s">
+      <c r="H26" s="17" t="s">
         <v>183</v>
       </c>
-      <c r="I26" t="s">
+      <c r="I26" s="17" t="s">
         <v>9</v>
       </c>
+      <c r="J26" s="17"/>
+      <c r="K26" s="17"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="A27" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="17">
         <v>8</v>
       </c>
-      <c r="F27" s="4">
+      <c r="F27" s="18">
         <v>0.16700000000000001</v>
       </c>
-      <c r="G27" s="5">
+      <c r="G27" s="19">
         <f t="shared" si="0"/>
         <v>1.3360000000000001</v>
       </c>
-      <c r="H27" t="s">
+      <c r="H27" s="17" t="s">
         <v>184</v>
       </c>
-      <c r="I27" t="s">
+      <c r="I27" s="17" t="s">
         <v>9</v>
       </c>
+      <c r="J27" s="17"/>
+      <c r="K27" s="17"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="A28" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="E28">
-        <v>1</v>
-      </c>
-      <c r="F28" s="4">
+      <c r="E28" s="17">
+        <v>1</v>
+      </c>
+      <c r="F28" s="18">
         <v>0.92100000000000004</v>
       </c>
-      <c r="G28" s="5">
+      <c r="G28" s="19">
         <f t="shared" si="0"/>
         <v>0.92100000000000004</v>
       </c>
-      <c r="H28" t="s">
+      <c r="H28" s="17" t="s">
         <v>185</v>
       </c>
-      <c r="I28" t="s">
+      <c r="I28" s="17" t="s">
         <v>9</v>
       </c>
+      <c r="J28" s="17"/>
+      <c r="K28" s="17"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="A29" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="17">
         <v>220</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="E29">
-        <v>1</v>
-      </c>
-      <c r="F29" s="4">
+      <c r="E29" s="17">
+        <v>1</v>
+      </c>
+      <c r="F29" s="18">
         <v>0.158</v>
       </c>
-      <c r="G29" s="5">
+      <c r="G29" s="19">
         <f t="shared" si="0"/>
         <v>0.158</v>
       </c>
-      <c r="H29" t="s">
+      <c r="H29" s="17" t="s">
         <v>186</v>
       </c>
-      <c r="I29" t="s">
+      <c r="I29" s="17" t="s">
         <v>9</v>
       </c>
+      <c r="J29" s="17"/>
+      <c r="K29" s="17"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="A30" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="17">
         <v>2</v>
       </c>
-      <c r="F30" s="4">
+      <c r="F30" s="18">
         <v>0.17699999999999999</v>
       </c>
-      <c r="G30" s="5">
+      <c r="G30" s="19">
         <f t="shared" si="0"/>
         <v>0.35399999999999998</v>
       </c>
-      <c r="H30" t="s">
+      <c r="H30" s="17" t="s">
         <v>187</v>
       </c>
-      <c r="I30" t="s">
+      <c r="I30" s="17" t="s">
         <v>9</v>
       </c>
+      <c r="J30" s="17"/>
+      <c r="K30" s="17"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="A31" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="17">
         <v>2</v>
       </c>
-      <c r="F31" s="4">
+      <c r="F31" s="18">
         <v>9.2999999999999999E-2</v>
       </c>
-      <c r="G31" s="5">
+      <c r="G31" s="19">
         <f t="shared" si="0"/>
         <v>0.186</v>
       </c>
-      <c r="H31" t="s">
+      <c r="H31" s="17" t="s">
         <v>188</v>
       </c>
-      <c r="I31" t="s">
+      <c r="I31" s="17" t="s">
         <v>9</v>
       </c>
+      <c r="J31" s="17"/>
+      <c r="K31" s="17"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="A32" s="17" t="s">
         <v>127</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="17">
         <v>2</v>
       </c>
-      <c r="F32" s="4">
+      <c r="F32" s="18">
         <v>9.2999999999999999E-2</v>
       </c>
-      <c r="G32" s="5">
+      <c r="G32" s="19">
         <f t="shared" si="0"/>
         <v>0.186</v>
       </c>
-      <c r="H32" t="s">
+      <c r="H32" s="17" t="s">
         <v>189</v>
       </c>
-      <c r="I32" t="s">
+      <c r="I32" s="17" t="s">
         <v>9</v>
       </c>
+      <c r="J32" s="17"/>
+      <c r="K32" s="17"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="A33" s="17" t="s">
         <v>129</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="E33">
-        <v>1</v>
-      </c>
-      <c r="F33" s="4">
+      <c r="E33" s="17">
+        <v>1</v>
+      </c>
+      <c r="F33" s="18">
         <v>2.0699999999999998</v>
       </c>
-      <c r="G33" s="5">
+      <c r="G33" s="19">
         <f t="shared" si="0"/>
         <v>2.0699999999999998</v>
       </c>
-      <c r="H33" s="3" t="s">
+      <c r="H33" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="I33" t="s">
+      <c r="I33" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="J33" t="s">
+      <c r="J33" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="K33" t="s">
+      <c r="K33" s="17" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="A34" s="17" t="s">
         <v>135</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="E34">
-        <v>1</v>
-      </c>
-      <c r="F34" s="4">
+      <c r="E34" s="17">
+        <v>1</v>
+      </c>
+      <c r="F34" s="18">
         <v>1.6</v>
       </c>
-      <c r="G34" s="5">
+      <c r="G34" s="19">
         <f t="shared" si="0"/>
         <v>1.6</v>
       </c>
-      <c r="H34" t="s">
+      <c r="H34" s="17" t="s">
         <v>163</v>
       </c>
+      <c r="I34" s="17"/>
+      <c r="J34" s="17"/>
+      <c r="K34" s="17"/>
     </row>
     <row r="35" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A35" s="6" t="s">
+      <c r="A35" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="7">
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="5">
         <f>SUM(G3:G34)</f>
         <v>71.418000000000021</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A36" s="6"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="7"/>
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="5"/>
     </row>
     <row r="37" spans="1:11" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="1" t="s">
@@ -2225,15 +2271,15 @@
       <c r="E38">
         <v>1</v>
       </c>
-      <c r="F38" s="5">
+      <c r="F38" s="3">
         <v>2</v>
       </c>
-      <c r="G38" s="5">
+      <c r="G38" s="3">
         <f>F38*E38</f>
         <v>2</v>
       </c>
-      <c r="H38" s="3" t="s">
-        <v>205</v>
+      <c r="H38" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -2243,14 +2289,14 @@
       <c r="E39">
         <v>1</v>
       </c>
-      <c r="F39" s="5">
+      <c r="F39" s="3">
         <v>6.11</v>
       </c>
-      <c r="G39" s="5">
+      <c r="G39" s="3">
         <f t="shared" ref="G39:G43" si="1">F39*E39</f>
         <v>6.11</v>
       </c>
-      <c r="H39" s="3" t="s">
+      <c r="H39" t="s">
         <v>167</v>
       </c>
     </row>
@@ -2261,14 +2307,14 @@
       <c r="E40">
         <v>1</v>
       </c>
-      <c r="F40" s="5">
+      <c r="F40" s="3">
         <v>2.12</v>
       </c>
-      <c r="G40" s="5">
+      <c r="G40" s="3">
         <f t="shared" si="1"/>
         <v>2.12</v>
       </c>
-      <c r="H40" s="3" t="s">
+      <c r="H40" t="s">
         <v>170</v>
       </c>
     </row>
@@ -2279,14 +2325,14 @@
       <c r="E41">
         <v>1</v>
       </c>
-      <c r="F41" s="5">
+      <c r="F41" s="3">
         <v>2.0099999999999998</v>
       </c>
-      <c r="G41" s="5">
+      <c r="G41" s="3">
         <f t="shared" si="1"/>
         <v>2.0099999999999998</v>
       </c>
-      <c r="H41" s="3" t="s">
+      <c r="H41" t="s">
         <v>192</v>
       </c>
     </row>
@@ -2297,14 +2343,14 @@
       <c r="E42">
         <v>1</v>
       </c>
-      <c r="F42" s="5">
+      <c r="F42" s="3">
         <v>2.4700000000000002</v>
       </c>
-      <c r="G42" s="5">
+      <c r="G42" s="3">
         <f t="shared" si="1"/>
         <v>2.4700000000000002</v>
       </c>
-      <c r="H42" s="3" t="s">
+      <c r="H42" t="s">
         <v>190</v>
       </c>
     </row>
@@ -2315,36 +2361,36 @@
       <c r="E43">
         <v>1</v>
       </c>
-      <c r="F43" s="5">
+      <c r="F43" s="3">
         <v>5</v>
       </c>
-      <c r="G43" s="5">
+      <c r="G43" s="3">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="H43" s="3" t="s">
-        <v>205</v>
+      <c r="H43" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A44" s="6" t="s">
+      <c r="A44" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="B44" s="6"/>
-      <c r="C44" s="6"/>
-      <c r="D44" s="6"/>
-      <c r="E44" s="6"/>
-      <c r="F44" s="6"/>
-      <c r="G44" s="7">
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="5">
         <f>SUM(G38:G43)</f>
         <v>19.71</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46" s="8" t="s">
+      <c r="A46" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="B46" s="8"/>
+      <c r="B46" s="11"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
@@ -2353,7 +2399,7 @@
       <c r="E47">
         <v>1</v>
       </c>
-      <c r="F47" s="5">
+      <c r="F47" s="3">
         <v>171.4</v>
       </c>
       <c r="G47">
@@ -2371,7 +2417,7 @@
       <c r="E48">
         <v>1</v>
       </c>
-      <c r="F48" s="5">
+      <c r="F48" s="3">
         <v>66.34</v>
       </c>
       <c r="G48">
@@ -2389,7 +2435,7 @@
       <c r="E49">
         <v>1</v>
       </c>
-      <c r="F49" s="5">
+      <c r="F49" s="3">
         <v>38.340000000000003</v>
       </c>
       <c r="G49">
@@ -2401,31 +2447,31 @@
       </c>
     </row>
     <row r="50" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A50" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="G50" s="7">
+      <c r="A50" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="G50" s="5">
         <f>SUM(G47:G49)</f>
         <v>276.08000000000004</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A52" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="B52" s="8"/>
-      <c r="C52" s="12" t="s">
-        <v>207</v>
+      <c r="A52" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="B52" s="11"/>
+      <c r="C52" s="7" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E53">
         <v>1</v>
       </c>
-      <c r="F53" s="5">
+      <c r="F53" s="3">
         <v>35.06</v>
       </c>
       <c r="G53">
@@ -2433,17 +2479,17 @@
         <v>35.06</v>
       </c>
       <c r="H53" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E54">
         <v>1</v>
       </c>
-      <c r="F54" s="5">
+      <c r="F54" s="3">
         <v>4.0199999999999996</v>
       </c>
       <c r="G54">
@@ -2451,40 +2497,40 @@
         <v>4.0199999999999996</v>
       </c>
       <c r="H54" t="s">
-        <v>195</v>
+        <v>207</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A55" s="11" t="s">
-        <v>198</v>
-      </c>
-      <c r="B55" s="11"/>
-      <c r="G55" s="7">
+      <c r="A55" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="B55" s="13"/>
+      <c r="G55" s="5">
         <f>SUM(G53:G54)</f>
         <v>39.08</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A56" s="6"/>
+      <c r="A56" s="4"/>
     </row>
     <row r="57" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A57" s="10" t="s">
+      <c r="A57" s="12" t="s">
         <v>194</v>
       </c>
-      <c r="B57" s="10"/>
-      <c r="C57" s="10"/>
-      <c r="G57" s="9">
+      <c r="B57" s="12"/>
+      <c r="C57" s="12"/>
+      <c r="G57" s="6">
         <f>G50+G44+G35</f>
         <v>367.20800000000003</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A58" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="B58" s="13"/>
-      <c r="C58" s="13"/>
-      <c r="G58" s="14">
+      <c r="A58" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="B58" s="10"/>
+      <c r="C58" s="10"/>
+      <c r="G58" s="8">
         <f>G55+G44+G35</f>
         <v>130.20800000000003</v>
       </c>
@@ -2505,8 +2551,10 @@
     <hyperlink ref="H33" r:id="rId5"/>
     <hyperlink ref="H40" r:id="rId6"/>
     <hyperlink ref="H25" r:id="rId7"/>
+    <hyperlink ref="H53" r:id="rId8"/>
+    <hyperlink ref="H54" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId8"/>
+  <pageSetup paperSize="9" scale="28" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>